<commit_message>
Jackie - Excel update
</commit_message>
<xml_diff>
--- a/documentation/Features/Features_Security_Testing.xlsx
+++ b/documentation/Features/Features_Security_Testing.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>#1</t>
   </si>
@@ -151,13 +151,40 @@
   </si>
   <si>
     <t xml:space="preserve">The image slider doesn’t display correctly across browsers and/or platforms.  In addition, the admin has trouble customizing what images are being shown and/or the speed of the animation.   </t>
+  </si>
+  <si>
+    <t>We will test to ensure the images and content that are picked within the timeline slider display properly.</t>
+  </si>
+  <si>
+    <t>The timeline slider display in proper order without errors</t>
+  </si>
+  <si>
+    <t>The images and contents do not advance through the sense, as they should. Display them out of the proper sequence without the designed interval; any of the images are not properly called from the database.</t>
+  </si>
+  <si>
+    <t>We will create a f&amp;q generator on the page that helps to identify patient’s health issue. The multiple choice form will consist of several radio buttons with the submissions posting back to the page using ajax to display aggregate result of overall submission.</t>
+  </si>
+  <si>
+    <t>The f&amp;q generator accepts the users input and successfully passes it to the database which return the suitable health assessment.</t>
+  </si>
+  <si>
+    <t>The generator doesn’t pass user input to database. It doesn’t display the result properly.</t>
+  </si>
+  <si>
+    <t>We will test to ensure the content are display properly</t>
+  </si>
+  <si>
+    <t>The content display in proper order without errors</t>
+  </si>
+  <si>
+    <t>The content do not advance thourh the sense as they should. Display them out of the properly sequence without the designed interval any of the images are not properly called from the database.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -187,6 +214,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
     </font>
   </fonts>
   <fills count="3">
@@ -223,7 +255,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -244,6 +276,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -592,23 +627,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="7" max="7" width="36.25" customWidth="1"/>
-    <col min="8" max="8" width="35.375" customWidth="1"/>
+    <col min="7" max="7" width="36.1640625" customWidth="1"/>
+    <col min="8" max="8" width="35.33203125" customWidth="1"/>
     <col min="9" max="9" width="25" customWidth="1"/>
-    <col min="11" max="11" width="12.125" customWidth="1"/>
-    <col min="12" max="12" width="13.625" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
     <col min="14" max="14" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="31.5">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -628,7 +663,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -672,22 +707,49 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="135">
       <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="105">
       <c r="D4" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="120">
       <c r="D5" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="G5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="135">
       <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
@@ -701,7 +763,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="236.25">
       <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
@@ -715,7 +777,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="173.25">
       <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
@@ -729,125 +791,125 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="31.5">
       <c r="D9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="D10" s="3" t="s">
         <v>24</v>
       </c>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="D11" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="D12" s="3" t="s">
         <v>26</v>
       </c>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="D13" s="3" t="s">
         <v>27</v>
       </c>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="31.5">
       <c r="D14" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14">
       <c r="D15" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14">
       <c r="D16" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4">
       <c r="D17" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4">
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4">
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4">
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4">
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:4">
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:4">
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:4">
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4">
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4">
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4">
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4">
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4">
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4">
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4">
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:4">
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4">
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4">
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4">
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4">
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4">
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4">
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4">
       <c r="D39" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Kate - UPDATE Security Testing Table
</commit_message>
<xml_diff>
--- a/documentation/Features/Features_Security_Testing.xlsx
+++ b/documentation/Features/Features_Security_Testing.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20740" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -19,7 +19,62 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+  <si>
+    <t>Applicants details were not successfully added to applicant table. Confirmation email was not sent to user. Administrators are unable to view the new applicants submission.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patients will be able to login using a username and password to view their appointment details. Doctors will be able to login and view appointments that are booked with them and to book new appointments with patients that have a username and password. Admininstrators will be able to change dashboard content but not appointment details.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patients are able to view their appointments. Doctors are able to add new appointments to the appointment table. Those new appointments are then viewable to the patient. The doctor is also able to view a listing of their appointments.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patients are not able to view any of their appointments. Doctors are not able to add in new apointments successfully to the appointment table. The new appointments added by doctors are not viewable to the patient. The doctor is not able to view his or her listing of appointments.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>After submission the user's details, resume and job selection will appear in the applicant table. The user will receive a confirmation email stating that their information was recevied and thanking them for their application. The administrator will be able to view the new applicants submission.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>User will be requested to fill out a form and upload a resume. The form will also require them to select the job they are applying for. User details along with their resume and job selection will be uploaded to the applicant table.A confirmation email will be sent to applicant. Administrators will be able to view the user information that has been submitted.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>The user can complete a form to join/subscribe to mailing list. The users details will then be sent to the mailingList table and stored there. A confirmation email will be sent to the user to confirm they have been added to the list. When unsubscribing, the user will be removed from the mailingList table. If they did not previously exist on the table a message will appear stating that they are not a subscriber.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>The user's details are visible within the mailingList table. A confirmation email has been successfully delivered to the new subscriber. Another test email was successfully sent to ensure user is receiving newsletter. When user unsubscribes they are no longer visible in the mailingList table.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>When subscribing, user was not successfully added to mailingList table. Confirmation email was not sent to user. When unsubscribing, user was not successfully removed from mailingList table</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The search feature does not display correct results when searching by name and/or department.  In addition, additional information from the database may be displayed which is not authorized by the staff. 
+   From the admin side, the admin has problems disabling certain search features, and/or certain disable features are still shown to the user. 
+</t>
+  </si>
+  <si>
+    <t>The search feature works correctly and allows the user to search by name and/or department.  The information for the doctors and/or staff is shown correctly, and in addition no additional information is given where not authorized by those staff.From the admin side, the admin can decide what criteria to filter the search by, as well as successfully disable certain information from being shown to the user.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  The user is shown an image slider that displays the currently featured images/pages.  The image slider should work correctly across browsers and platforms, and render the animation in a clean and smooth manner. 
+  From the admin side, the admin can decide what images to show as well as customize the type and speed of the animation. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  The image slider works correctly by displaying uniformly across browsers and platforms.  The animation works smoothly and cleanly.  From the admin side, the admin is able to customize different pictures and the speed of the animation. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The image slider doesn’t display correctly across browsers and/or platforms.  In addition, the admin has trouble customizing what images are being shown and/or the speed of the animation.   </t>
+  </si>
   <si>
     <t>#1</t>
   </si>
@@ -132,32 +187,13 @@
     <t xml:space="preserve">Test to make sure the search feature works correctly.  The user is able to search either by doctor name, or by department, and the correct doctors show up alongside the correct contact information.  Additional information is not given out where not authorized by those doctors or faculty staff.
   From the admin side, the staff can decide what criteria to allow the user to search by, and to make sure they can disable certain information (such as cellphone) from being displayed to the user on the front end. 
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The search feature does not display correct results when searching by name and/or department.  In addition, additional information from the database may be displayed which is not authorized by the staff. 
-   From the admin side, the admin has problems disabling certain search features, and/or certain disable features are still shown to the user. 
-</t>
-  </si>
-  <si>
-    <t>The search feature works correctly and allows the user to search by name and/or department.  The information for the doctors and/or staff is shown correctly, and in addition no additional information is given where not authorized by those staff.From the admin side, the admin can decide what criteria to filter the search by, as well as successfully disable certain information from being shown to the user.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  The user is shown an image slider that displays the currently featured images/pages.  The image slider should work correctly across browsers and platforms, and render the animation in a clean and smooth manner. 
-  From the admin side, the admin can decide what images to show as well as customize the type and speed of the animation. 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  The image slider works correctly by displaying uniformly across browsers and platforms.  The animation works smoothly and cleanly.  From the admin side, the admin is able to customize different pictures and the speed of the animation. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The image slider doesn’t display correctly across browsers and/or platforms.  In addition, the admin has trouble customizing what images are being shown and/or the speed of the animation.   </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -188,6 +224,10 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -212,19 +252,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
@@ -246,20 +283,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -589,267 +623,292 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="7" max="7" width="36.25" customWidth="1"/>
-    <col min="8" max="8" width="35.375" customWidth="1"/>
+    <col min="7" max="7" width="36.1640625" customWidth="1"/>
+    <col min="8" max="8" width="35.33203125" customWidth="1"/>
     <col min="9" max="9" width="25" customWidth="1"/>
-    <col min="11" max="11" width="12.125" customWidth="1"/>
-    <col min="12" max="12" width="13.625" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
     <col min="14" max="14" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14">
+      <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="4" t="s">
+      <c r="B2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="D3" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="D4" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="D5" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="135">
+      <c r="D6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="225">
+      <c r="D7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="165">
+      <c r="D8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="30">
+      <c r="D9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="D10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="D11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:14" ht="165">
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="135">
+      <c r="D13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="14" spans="1:14" ht="165">
+      <c r="D14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="I14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D4" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="D6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="236.25" x14ac:dyDescent="0.25">
-      <c r="D7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="173.25" x14ac:dyDescent="0.25">
-      <c r="D8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D14" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D15" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D16" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D39" s="3"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="D15" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="D16" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="4:4">
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="4:4">
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="4:4">
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="4:4">
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="4:4">
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="4:4">
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="4:4">
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="4:4">
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="4:4">
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="4:4">
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="4:4">
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="4:4">
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="4:4">
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="4:4">
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="4:4">
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="4:4">
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="4:4">
+      <c r="D39" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Jackie - xlxx update
</commit_message>
<xml_diff>
--- a/documentation/Features/Features_Security_Testing.xlsx
+++ b/documentation/Features/Features_Security_Testing.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20740" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="4140" yWindow="0" windowWidth="23720" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Applicants details were not successfully added to applicant table. Confirmation email was not sent to user. Administrators are unable to view the new applicants submission.</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -187,13 +187,40 @@
     <t xml:space="preserve">Test to make sure the search feature works correctly.  The user is able to search either by doctor name, or by department, and the correct doctors show up alongside the correct contact information.  Additional information is not given out where not authorized by those doctors or faculty staff.
   From the admin side, the staff can decide what criteria to allow the user to search by, and to make sure they can disable certain information (such as cellphone) from being displayed to the user on the front end. 
 </t>
+  </si>
+  <si>
+    <t>We will test to ensure the images and content that are placed within the history timeline display properly</t>
+  </si>
+  <si>
+    <t>The timeline slider display in the proper order withotu any error</t>
+  </si>
+  <si>
+    <t>The images and content do not advnace through the series as they should, display them out of the proper sequence, without the disiignated interval, any of the image are not properly called from the database.</t>
+  </si>
+  <si>
+    <t>We will ensure the message that are place within the alert display properly</t>
+  </si>
+  <si>
+    <t>The alert display in the proper order without any error</t>
+  </si>
+  <si>
+    <t>The message do not advnace through the series as it should, display it out of the proper sequence, without the disiignated interval, any of the message are not properly called from the database.</t>
+  </si>
+  <si>
+    <t>We will input a few symptom in to the database and the appropriate symptom will display base on the user's f&amp;q input</t>
+  </si>
+  <si>
+    <t>The appropriate symptom display successfully base on the user's input</t>
+  </si>
+  <si>
+    <t>The symptom fail to display</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -293,7 +320,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -623,14 +650,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.1640625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
@@ -706,19 +733,46 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" ht="120">
       <c r="D3" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="G3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="45">
       <c r="D4" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="G4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="120">
       <c r="D5" s="4" t="s">
         <v>33</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="135">
@@ -908,7 +962,7 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Justin - file modified
</commit_message>
<xml_diff>
--- a/documentation/Features/Features_Security_Testing.xlsx
+++ b/documentation/Features/Features_Security_Testing.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="0" windowWidth="23720" windowHeight="15840" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Applicants details were not successfully added to applicant table. Confirmation email was not sent to user. Administrators are unable to view the new applicants submission.</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -214,6 +214,33 @@
   </si>
   <si>
     <t>The symptom fail to display</t>
+  </si>
+  <si>
+    <t>We'll test the donation system to make sure a user can make a donation online via the donation form and then be emailed a receipt. The user will complete the form using the name Dave Davidson, with dryden_dave_test@gmail.com as the email address and a test credit card account. The user will submit the donation form and test for success. The user will then check the email account to ensure the receipt arrives. The user will also ensure the data has been inserted into the database.</t>
+  </si>
+  <si>
+    <t>Proper validation of the form, the payment is secure and the transaction only occurs if all validation methods are met, the receipt is emailed to the donor, and all of the information is inserted into the database. The feature is responsive and works on all browsers.</t>
+  </si>
+  <si>
+    <t>The transaction doesn't go through, the transaction goes through multiple times, validation doesn't occur, transaction not secure, information doesn't get stored in the database, no receipt is emailed. The page isn't responsive and/or doesn't work on all browsers.</t>
+  </si>
+  <si>
+    <t>We'll test the e-card template that will allow users to send an e-card to a patient at the hospital. We'll test by having a user enter a name and an email adress of dryden_dave_test@gmail.com as the patients' email. The user will then fill out a greeting and customize the card with their choice of background and font. The user will then send the card and be greeted with a success message. The user will then check the email to see if the card was successfully sent and appears as designed. The user will then test by using improper information and blank fields to ensure all error messages appear and ensure it does not send.</t>
+  </si>
+  <si>
+    <t>The user is successfully able to send an e-card they designed, the user receives a success message upon sending the card, proper validation occurs and errors occur when fields aren't filled in properly or left blank. The feature is responsive and works on all browsers.</t>
+  </si>
+  <si>
+    <t>Validation doesn't work as designed, e-card isn't sent, e-card isn't as designed, page is not responsive and/or doesn't work on all browsers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We'll test the  control of the patient survey to make sure the steps allow the user to go forward and backwards appropriately, proper validation controls and messages occur, and that the results are stored in the database. The user will go through the survey and then submit, and test for a success message. After a successful message, we will verify the answers were submitted into the database. The user will do the survey again, but this time leave questions unanswered and submit. Testing if the appropriate error messages appear. </t>
+  </si>
+  <si>
+    <t>The wizard control functions as designed with the buttons and controls, as well as displaying the proper error messages and the results are successfully inserted into the database. The user receives a thank you message thanking them for their feedback upon successful completion of the survey.The feature is responsive and works on all browsers.</t>
+  </si>
+  <si>
+    <t>The wizard control does not provide proper functionality, accepts invalid input, does not display error messages, and does not store the data in the database, page is not responsive and/or doesn't work on all browsers.</t>
   </si>
 </sst>
 </file>
@@ -653,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -877,64 +904,91 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" ht="195">
       <c r="D15" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="G15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="240">
       <c r="D16" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="4:4">
+      <c r="G16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" ht="195">
       <c r="D17" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="4:4">
+      <c r="G17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9">
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="4:4">
+    <row r="19" spans="4:9">
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="4:4">
+    <row r="20" spans="4:9">
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="4:4">
+    <row r="21" spans="4:9">
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="4:4">
+    <row r="22" spans="4:9">
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="4:4">
+    <row r="23" spans="4:9">
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="4:4">
+    <row r="24" spans="4:9">
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="4:4">
+    <row r="25" spans="4:9">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="4:4">
+    <row r="26" spans="4:9">
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="4:4">
+    <row r="27" spans="4:9">
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="4:4">
+    <row r="28" spans="4:9">
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="4:4">
+    <row r="29" spans="4:9">
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="4:4">
+    <row r="30" spans="4:9">
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="4:4">
+    <row r="31" spans="4:9">
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="4:4">
+    <row r="32" spans="4:9">
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="4:4">

</xml_diff>